<commit_message>
Modification du script ACP
</commit_message>
<xml_diff>
--- a/Km_data.xlsx
+++ b/Km_data.xlsx
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="O158" sqref="O158"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,7 +1590,7 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Amélioration ACP + plots
</commit_message>
<xml_diff>
--- a/Km_data.xlsx
+++ b/Km_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="198">
   <si>
     <t>Nom</t>
   </si>
@@ -499,9 +499,6 @@
   </si>
   <si>
     <t>Chatoon</t>
-  </si>
-  <si>
-    <t>Lokai</t>
   </si>
   <si>
     <t>TimeoGnc</t>
@@ -957,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="M130" sqref="M130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,7 +1301,7 @@
         <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -5953,7 +5950,7 @@
         <v>148</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C134">
         <v>7</v>
@@ -6278,7 +6275,7 @@
         <v>8</v>
       </c>
       <c r="D142" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F142">
         <v>0</v>
@@ -6304,16 +6301,16 @@
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>160</v>
+      </c>
+      <c r="B143">
+        <v>1</v>
+      </c>
+      <c r="C143">
+        <v>8</v>
+      </c>
+      <c r="D143" t="s">
         <v>161</v>
-      </c>
-      <c r="B143">
-        <v>1</v>
-      </c>
-      <c r="C143">
-        <v>8</v>
-      </c>
-      <c r="D143" t="s">
-        <v>162</v>
       </c>
       <c r="F143">
         <v>0</v>
@@ -6339,16 +6336,16 @@
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>162</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
+      <c r="C144">
+        <v>8</v>
+      </c>
+      <c r="D144" t="s">
         <v>163</v>
-      </c>
-      <c r="B144">
-        <v>1</v>
-      </c>
-      <c r="C144">
-        <v>8</v>
-      </c>
-      <c r="D144" t="s">
-        <v>164</v>
       </c>
       <c r="F144">
         <v>0</v>
@@ -6374,19 +6371,19 @@
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>164</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+      <c r="C145">
+        <v>8</v>
+      </c>
+      <c r="D145" t="s">
+        <v>163</v>
+      </c>
+      <c r="E145" t="s">
         <v>165</v>
-      </c>
-      <c r="B145">
-        <v>1</v>
-      </c>
-      <c r="C145">
-        <v>8</v>
-      </c>
-      <c r="D145" t="s">
-        <v>164</v>
-      </c>
-      <c r="E145" t="s">
-        <v>166</v>
       </c>
       <c r="F145">
         <v>0</v>
@@ -6412,7 +6409,7 @@
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -6421,10 +6418,10 @@
         <v>8</v>
       </c>
       <c r="D146" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E146" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F146">
         <v>0</v>
@@ -6450,19 +6447,19 @@
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>167</v>
+      </c>
+      <c r="B147">
+        <v>1</v>
+      </c>
+      <c r="C147">
+        <v>8</v>
+      </c>
+      <c r="D147" t="s">
+        <v>161</v>
+      </c>
+      <c r="E147" t="s">
         <v>168</v>
-      </c>
-      <c r="B147">
-        <v>1</v>
-      </c>
-      <c r="C147">
-        <v>8</v>
-      </c>
-      <c r="D147" t="s">
-        <v>162</v>
-      </c>
-      <c r="E147" t="s">
-        <v>169</v>
       </c>
       <c r="F147">
         <v>1</v>
@@ -6488,7 +6485,7 @@
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -6497,10 +6494,10 @@
         <v>8</v>
       </c>
       <c r="D148" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E148" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F148">
         <v>1</v>
@@ -6509,7 +6506,7 @@
         <v>10</v>
       </c>
       <c r="H148" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I148">
         <v>3</v>
@@ -6529,7 +6526,7 @@
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B149">
         <v>1</v>
@@ -6538,10 +6535,10 @@
         <v>8</v>
       </c>
       <c r="D149" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E149" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F149">
         <v>1</v>
@@ -6576,10 +6573,10 @@
         <v>8</v>
       </c>
       <c r="D150" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E150" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F150">
         <v>1</v>
@@ -6605,7 +6602,7 @@
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B151">
         <v>1</v>
@@ -6614,10 +6611,10 @@
         <v>8</v>
       </c>
       <c r="D151" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E151" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F151">
         <v>1</v>
@@ -6652,10 +6649,10 @@
         <v>8</v>
       </c>
       <c r="D152" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E152" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F152">
         <v>1</v>
@@ -6664,7 +6661,7 @@
         <v>6</v>
       </c>
       <c r="H152" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I152">
         <v>0</v>
@@ -6684,7 +6681,7 @@
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B153">
         <v>1</v>
@@ -6693,10 +6690,10 @@
         <v>8</v>
       </c>
       <c r="D153" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E153" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F153">
         <v>1</v>
@@ -6722,7 +6719,7 @@
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B154">
         <v>1</v>
@@ -6731,10 +6728,10 @@
         <v>8</v>
       </c>
       <c r="D154" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E154" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F154">
         <v>1</v>
@@ -6760,7 +6757,7 @@
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B155">
         <v>1</v>
@@ -6769,10 +6766,10 @@
         <v>8</v>
       </c>
       <c r="D155" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E155" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F155">
         <v>1</v>
@@ -6798,7 +6795,7 @@
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B156">
         <v>1</v>
@@ -6807,10 +6804,10 @@
         <v>8</v>
       </c>
       <c r="D156" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E156" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F156">
         <v>1</v>
@@ -6836,7 +6833,7 @@
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B157">
         <v>1</v>
@@ -6845,10 +6842,10 @@
         <v>8</v>
       </c>
       <c r="D157" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E157" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F157">
         <v>1</v>
@@ -6874,7 +6871,7 @@
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B158">
         <v>1</v>
@@ -6883,10 +6880,10 @@
         <v>9</v>
       </c>
       <c r="D158" t="s">
+        <v>179</v>
+      </c>
+      <c r="E158" t="s">
         <v>180</v>
-      </c>
-      <c r="E158" t="s">
-        <v>181</v>
       </c>
       <c r="F158">
         <v>0</v>
@@ -6912,7 +6909,7 @@
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B159">
         <v>1</v>
@@ -6921,7 +6918,7 @@
         <v>9</v>
       </c>
       <c r="D159" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F159">
         <v>0</v>
@@ -6947,7 +6944,7 @@
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B160">
         <v>1</v>
@@ -6956,7 +6953,7 @@
         <v>9</v>
       </c>
       <c r="D160" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F160">
         <v>0</v>
@@ -6982,7 +6979,7 @@
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B161">
         <v>1</v>
@@ -6991,10 +6988,10 @@
         <v>9</v>
       </c>
       <c r="D161" t="s">
+        <v>184</v>
+      </c>
+      <c r="E161" t="s">
         <v>185</v>
-      </c>
-      <c r="E161" t="s">
-        <v>186</v>
       </c>
       <c r="F161">
         <v>0</v>
@@ -7029,10 +7026,10 @@
         <v>9</v>
       </c>
       <c r="D162" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E162" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F162">
         <v>0</v>
@@ -7058,7 +7055,7 @@
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B163">
         <v>1</v>
@@ -7067,10 +7064,10 @@
         <v>9</v>
       </c>
       <c r="D163" t="s">
+        <v>179</v>
+      </c>
+      <c r="E163" t="s">
         <v>180</v>
-      </c>
-      <c r="E163" t="s">
-        <v>181</v>
       </c>
       <c r="F163">
         <v>0</v>
@@ -7096,7 +7093,7 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B164">
         <v>1</v>
@@ -7105,10 +7102,10 @@
         <v>9</v>
       </c>
       <c r="D164" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E164" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F164">
         <v>1</v>
@@ -7140,16 +7137,16 @@
         <v>73</v>
       </c>
       <c r="B165">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C165">
         <v>9</v>
       </c>
       <c r="D165" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E165" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F165">
         <v>1</v>
@@ -7175,7 +7172,7 @@
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B166">
         <v>1</v>
@@ -7184,10 +7181,10 @@
         <v>9</v>
       </c>
       <c r="D166" t="s">
+        <v>184</v>
+      </c>
+      <c r="E166" t="s">
         <v>185</v>
-      </c>
-      <c r="E166" t="s">
-        <v>186</v>
       </c>
       <c r="F166">
         <v>1</v>
@@ -7213,7 +7210,7 @@
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B167">
         <v>1</v>
@@ -7222,10 +7219,10 @@
         <v>9</v>
       </c>
       <c r="D167" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E167" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F167">
         <v>1</v>
@@ -7234,7 +7231,7 @@
         <v>7</v>
       </c>
       <c r="H167" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I167">
         <v>2</v>
@@ -7254,7 +7251,7 @@
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B168">
         <v>1</v>
@@ -7263,10 +7260,10 @@
         <v>9</v>
       </c>
       <c r="D168" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E168" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F168">
         <v>1</v>
@@ -7292,7 +7289,7 @@
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B169">
         <v>1</v>
@@ -7301,10 +7298,10 @@
         <v>9</v>
       </c>
       <c r="D169" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E169" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F169">
         <v>1</v>
@@ -7330,7 +7327,7 @@
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B170">
         <v>1</v>
@@ -7339,10 +7336,10 @@
         <v>9</v>
       </c>
       <c r="D170" t="s">
+        <v>184</v>
+      </c>
+      <c r="E170" t="s">
         <v>185</v>
-      </c>
-      <c r="E170" t="s">
-        <v>186</v>
       </c>
       <c r="F170">
         <v>1</v>
@@ -7377,10 +7374,10 @@
         <v>9</v>
       </c>
       <c r="D171" t="s">
+        <v>184</v>
+      </c>
+      <c r="E171" t="s">
         <v>185</v>
-      </c>
-      <c r="E171" t="s">
-        <v>186</v>
       </c>
       <c r="F171">
         <v>1</v>
@@ -7406,7 +7403,7 @@
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B172">
         <v>1</v>
@@ -7415,10 +7412,10 @@
         <v>9</v>
       </c>
       <c r="D172" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E172" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F172">
         <v>1</v>
@@ -7427,7 +7424,7 @@
         <v>2</v>
       </c>
       <c r="H172" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I172">
         <v>2</v>
@@ -7456,10 +7453,10 @@
         <v>9</v>
       </c>
       <c r="D173" t="s">
+        <v>179</v>
+      </c>
+      <c r="E173" t="s">
         <v>180</v>
-      </c>
-      <c r="E173" t="s">
-        <v>181</v>
       </c>
       <c r="F173">
         <v>1</v>

</xml_diff>